<commit_message>
normalized 2017 2018 org c fluxes to 100 m no diff
</commit_message>
<xml_diff>
--- a/data/flux/2019-fluxes.xlsx
+++ b/data/flux/2019-fluxes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="70">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t xml:space="preserve">*in prep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized to 100 m</t>
   </si>
 </sst>
 </file>
@@ -237,11 +240,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -260,6 +264,11 @@
     </font>
     <font>
       <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -469,6 +478,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -570,11 +580,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="68815586"/>
-        <c:axId val="62662936"/>
+        <c:axId val="67745424"/>
+        <c:axId val="15818416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68815586"/>
+        <c:axId val="67745424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -608,7 +618,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -630,12 +640,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62662936"/>
+        <c:crossAx val="15818416"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62662936"/>
+        <c:axId val="15818416"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -678,7 +688,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -700,9 +710,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68815586"/>
+        <c:crossAx val="67745424"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -829,6 +839,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -948,11 +959,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1006513"/>
-        <c:axId val="39058567"/>
+        <c:axId val="89353219"/>
+        <c:axId val="60328809"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1006513"/>
+        <c:axId val="89353219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -986,7 +997,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1008,12 +1019,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39058567"/>
+        <c:crossAx val="60328809"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39058567"/>
+        <c:axId val="60328809"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1056,7 +1067,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1078,9 +1089,749 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006513"/>
+        <c:crossAx val="89353219"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2019 P3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.941818736708984</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.58022444076048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.658384034444609</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.379446369022148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.409333060179146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.770693405050107</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.482623052893713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.431731567122859</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="67269862"/>
+        <c:axId val="16322571"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="67269862"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (umol C/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16322571"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="16322571"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67269862"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2019 P2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$13:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>14.2603739269038</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.667837665365805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81767154976611</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.23184483190041</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.899087924837326</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.13759182314207</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.867361889808575</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.38881261783336</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.833874122781965</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.50161052021609</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.747473372001856</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$13:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="64925089"/>
+        <c:axId val="32450495"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64925089"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (umol/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="32450495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="32450495"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64925089"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1130,16 +1881,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>488520</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>164520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>121680</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>402480</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1147,8 +1898,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5590440" y="200880"/>
-        <a:ext cx="5322960" cy="4283640"/>
+        <a:off x="4457520" y="47880"/>
+        <a:ext cx="5122440" cy="4283280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1160,16 +1911,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>617400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>77760</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>408960</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>186480</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1177,12 +1928,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5719320" y="4580280"/>
-        <a:ext cx="5481360" cy="5221080"/>
+        <a:off x="4370760" y="4513320"/>
+        <a:ext cx="4993200" cy="5220720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>507240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>48240</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>153000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="9684720" y="28800"/>
+        <a:ext cx="4425480" cy="4513320"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>303480</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>124200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>412200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>143280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="9480960" y="4513320"/>
+        <a:ext cx="4993200" cy="5220720"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1202,7 +2013,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="70.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.04"/>
@@ -2677,13 +3488,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M64" activeCellId="0" sqref="M64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>
@@ -2700,6 +3511,9 @@
       <c r="C1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -2711,6 +3525,10 @@
       <c r="C2" s="0" t="n">
         <v>38.90881844</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">C2/$C$2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -2722,6 +3540,10 @@
       <c r="C3" s="0" t="n">
         <v>36.64505423</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">C3/$C$2</f>
+        <v>0.941818736708984</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -2733,6 +3555,10 @@
       <c r="C4" s="0" t="n">
         <v>100.3934843</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">C4/$C$2</f>
+        <v>2.58022444076048</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -2744,6 +3570,10 @@
       <c r="C5" s="0" t="n">
         <v>25.61694486</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">C5/$C$2</f>
+        <v>0.658384034444609</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -2755,6 +3585,10 @@
       <c r="C6" s="0" t="n">
         <v>14.76380988</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">C6/$C$2</f>
+        <v>0.379446369022148</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2766,6 +3600,10 @@
       <c r="C7" s="0" t="n">
         <v>15.92666572</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">C7/$C$2</f>
+        <v>0.409333060179146</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -2777,6 +3615,10 @@
       <c r="C8" s="0" t="n">
         <v>29.98676977</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">C8/$C$2</f>
+        <v>0.770693405050107</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -2788,6 +3630,10 @@
       <c r="C9" s="0" t="n">
         <v>18.77829274</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">C9/$C$2</f>
+        <v>0.482623052893713</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -2799,6 +3645,10 @@
       <c r="C10" s="0" t="n">
         <v>16.79816516</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">C10/$C$2</f>
+        <v>0.431731567122859</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -2821,6 +3671,10 @@
       <c r="C13" s="0" t="n">
         <v>353.5566298</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">C13/$C$14</f>
+        <v>14.2603739269038</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -2832,6 +3686,10 @@
       <c r="C14" s="0" t="n">
         <v>24.79294243</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">C14/$C$14</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -2843,6 +3701,10 @@
       <c r="C15" s="0" t="n">
         <v>16.55766079</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">C15/$C$14</f>
+        <v>0.667837665365805</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -2854,6 +3716,10 @@
       <c r="C16" s="0" t="n">
         <v>45.06542609</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">C16/$C$14</f>
+        <v>1.81767154976611</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -2865,6 +3731,10 @@
       <c r="C17" s="0" t="n">
         <v>30.541058</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">C17/$C$14</f>
+        <v>1.23184483190041</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -2876,6 +3746,10 @@
       <c r="C18" s="0" t="n">
         <v>22.29103516</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">C18/$C$14</f>
+        <v>0.899087924837326</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -2887,6 +3761,10 @@
       <c r="C19" s="0" t="n">
         <v>52.99719101</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">C19/$C$14</f>
+        <v>2.13759182314207</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -2898,6 +3776,10 @@
       <c r="C20" s="0" t="n">
         <v>21.5044534</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">C20/$C$14</f>
+        <v>0.867361889808575</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -2909,6 +3791,10 @@
       <c r="C21" s="0" t="n">
         <v>34.43275128</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">C21/$C$14</f>
+        <v>1.38881261783336</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -2920,6 +3806,10 @@
       <c r="C22" s="0" t="n">
         <v>20.67419312</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">C22/$C$14</f>
+        <v>0.833874122781965</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -2931,6 +3821,10 @@
       <c r="C23" s="0" t="n">
         <v>86.81522804</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">C23/$C$14</f>
+        <v>3.50161052021609</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -2941,6 +3835,10 @@
       </c>
       <c r="C24" s="0" t="n">
         <v>18.53206428</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">C24/$C$14</f>
+        <v>0.747473372001856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed csv output of rr 2018 joined csvs
</commit_message>
<xml_diff>
--- a/data/flux/2019-fluxes.xlsx
+++ b/data/flux/2019-fluxes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="77">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">Station</t>
   </si>
   <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
     <t xml:space="preserve">Depth (m)</t>
   </si>
   <si>
@@ -54,6 +57,15 @@
   </si>
   <si>
     <t xml:space="preserve">Protein/org C of flux (ug protein/umol C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N production rate (nM N/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d15N vs Air N2 (permil)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d13C vs VPDB (permil)</t>
   </si>
   <si>
     <t xml:space="preserve">1-58_170m_NO2_ctl</t>
@@ -246,9 +258,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -330,13 +341,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -411,7 +426,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -594,11 +609,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="61044373"/>
-        <c:axId val="75582272"/>
+        <c:axId val="32887941"/>
+        <c:axId val="63272554"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61044373"/>
+        <c:axId val="32887941"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,12 +669,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75582272"/>
+        <c:crossAx val="63272554"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75582272"/>
+        <c:axId val="63272554"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -724,7 +739,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61044373"/>
+        <c:crossAx val="32887941"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -772,7 +787,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -973,11 +988,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="42861955"/>
-        <c:axId val="42528037"/>
+        <c:axId val="29278975"/>
+        <c:axId val="46560285"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42861955"/>
+        <c:axId val="29278975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,12 +1048,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42528037"/>
+        <c:crossAx val="46560285"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42528037"/>
+        <c:axId val="46560285"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1103,7 +1118,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42861955"/>
+        <c:crossAx val="29278975"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1151,7 +1166,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1367,11 +1382,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="50526733"/>
-        <c:axId val="32528029"/>
+        <c:axId val="11703092"/>
+        <c:axId val="31850033"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50526733"/>
+        <c:axId val="11703092"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1427,12 +1442,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32528029"/>
+        <c:crossAx val="31850033"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32528029"/>
+        <c:axId val="31850033"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1497,7 +1512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50526733"/>
+        <c:crossAx val="11703092"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1545,7 +1560,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1746,11 +1761,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="67306284"/>
-        <c:axId val="2161304"/>
+        <c:axId val="13217630"/>
+        <c:axId val="80376665"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67306284"/>
+        <c:axId val="13217630"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1806,12 +1821,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2161304"/>
+        <c:crossAx val="80376665"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2161304"/>
+        <c:axId val="80376665"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1876,7 +1891,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67306284"/>
+        <c:crossAx val="13217630"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1935,9 +1950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>401760</xdr:colOff>
+      <xdr:colOff>401400</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1945,8 +1960,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4465080" y="47880"/>
-        <a:ext cx="5136840" cy="4282560"/>
+        <a:off x="4469040" y="47880"/>
+        <a:ext cx="5144040" cy="4282200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1965,9 +1980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>185760</xdr:colOff>
+      <xdr:colOff>185400</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1975,8 +1990,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4378320" y="4513320"/>
-        <a:ext cx="5007600" cy="5220000"/>
+        <a:off x="4382280" y="4513320"/>
+        <a:ext cx="5014800" cy="5219640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1995,9 +2010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>47520</xdr:colOff>
+      <xdr:colOff>47160</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2005,8 +2020,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9707400" y="28800"/>
-        <a:ext cx="4440240" cy="4512600"/>
+        <a:off x="9718920" y="28800"/>
+        <a:ext cx="4447440" cy="4512240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2025,9 +2040,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:colOff>411120</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2035,8 +2050,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9503640" y="4513320"/>
-        <a:ext cx="5007960" cy="5220000"/>
+        <a:off x="9515160" y="4513320"/>
+        <a:ext cx="5015160" cy="5219640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2054,28 +2069,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K107"/>
+  <dimension ref="A1:O107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1014" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2109,13 +2114,25 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>2019</v>
@@ -2123,22 +2140,22 @@
       <c r="D2" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="0" t="n">
         <v>170</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>7.75319567354966</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2019</v>
@@ -2146,11 +2163,11 @@
       <c r="D3" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="0" t="n">
         <v>170</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>14.62984724</v>
@@ -2170,10 +2187,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2019</v>
@@ -2181,22 +2198,22 @@
       <c r="D4" s="0" t="n">
         <v>570</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="0" t="n">
         <v>570</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>3.6622641509434</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2019</v>
@@ -2204,11 +2221,11 @@
       <c r="D5" s="0" t="n">
         <v>570</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="0" t="n">
         <v>570</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>41.66411217</v>
@@ -2228,10 +2245,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2019</v>
@@ -2239,22 +2256,22 @@
       <c r="D6" s="0" t="n">
         <v>570</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="0" t="n">
         <v>570</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>9.72617743702081</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2019</v>
@@ -2262,22 +2279,22 @@
       <c r="D7" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="0" t="n">
         <v>370</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>1.85815047021944</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2019</v>
@@ -2285,11 +2302,11 @@
       <c r="D8" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="0" t="n">
         <v>370</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>19.66438915</v>
@@ -2309,10 +2326,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>2019</v>
@@ -2320,22 +2337,22 @@
       <c r="D9" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="0" t="n">
         <v>370</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>6.57961447055717</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>2019</v>
@@ -2343,22 +2360,22 @@
       <c r="D10" s="0" t="n">
         <v>102</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="0" t="n">
         <v>102</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>24.9704142011834</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>2019</v>
@@ -2366,11 +2383,11 @@
       <c r="D11" s="0" t="n">
         <v>102</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="0" t="n">
         <v>102</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>31.44875954</v>
@@ -2390,10 +2407,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2019</v>
@@ -2401,22 +2418,22 @@
       <c r="D12" s="0" t="n">
         <v>102</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="0" t="n">
         <v>102</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>9.5391061452514</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2019</v>
@@ -2424,11 +2441,11 @@
       <c r="D13" s="0" t="n">
         <v>770</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="0" t="n">
         <v>770</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>20.11954101</v>
@@ -2448,10 +2465,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>2019</v>
@@ -2459,22 +2476,22 @@
       <c r="D14" s="0" t="n">
         <v>770</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="0" t="n">
         <v>770</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>11.0183881064163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2019</v>
@@ -2482,22 +2499,22 @@
       <c r="D15" s="0" t="n">
         <v>770</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="0" t="n">
         <v>770</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>7.13300230537329</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2019</v>
@@ -2505,11 +2522,11 @@
       <c r="D16" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="0" t="n">
         <v>130</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>54.59667624</v>
@@ -2529,10 +2546,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2019</v>
@@ -2540,22 +2557,22 @@
       <c r="D17" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="0" t="n">
         <v>130</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>10.0321931589537</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2019</v>
@@ -2563,22 +2580,22 @@
       <c r="D18" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="0" t="n">
         <v>130</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>25.396694214876</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>2019</v>
@@ -2586,11 +2603,11 @@
       <c r="D19" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="0" t="n">
         <v>300</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>82.77252678</v>
@@ -2610,10 +2627,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>2019</v>
@@ -2621,11 +2638,11 @@
       <c r="D20" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>61.24302838</v>
@@ -2645,10 +2662,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>2019</v>
@@ -2656,22 +2673,22 @@
       <c r="D21" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>11.1135940409683</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>2019</v>
@@ -2679,22 +2696,22 @@
       <c r="D22" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>12.3389830508475</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>2019</v>
@@ -2702,11 +2719,11 @@
       <c r="D23" s="0" t="n">
         <v>965</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="0" t="n">
         <v>965</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>51.08955421</v>
@@ -2726,10 +2743,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>2019</v>
@@ -2737,22 +2754,22 @@
       <c r="D24" s="0" t="n">
         <v>965</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="0" t="n">
         <v>965</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>12.3266761768902</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>2019</v>
@@ -2760,22 +2777,22 @@
       <c r="D25" s="0" t="n">
         <v>965</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="0" t="n">
         <v>965</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>35.8697318007663</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>2019</v>
@@ -2783,11 +2800,11 @@
       <c r="D26" s="0" t="n">
         <v>173</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="0" t="n">
         <v>173</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>53.1000796</v>
@@ -2807,10 +2824,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>2019</v>
@@ -2818,22 +2835,22 @@
       <c r="D27" s="0" t="n">
         <v>173</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="0" t="n">
         <v>173</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G27" s="0" t="n">
         <v>29.8271604938272</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>2019</v>
@@ -2841,22 +2858,22 @@
       <c r="D28" s="0" t="n">
         <v>173</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="0" t="n">
         <v>173</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G28" s="0" t="n">
         <v>14.1515151515152</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>2019</v>
@@ -2864,11 +2881,11 @@
       <c r="D29" s="0" t="n">
         <v>965</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="0" t="n">
         <v>965</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>21.16318464</v>
@@ -2888,10 +2905,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>2019</v>
@@ -2899,22 +2916,22 @@
       <c r="D30" s="0" t="n">
         <v>402</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="0" t="n">
         <v>402</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G30" s="0" t="n">
         <v>30.1541353383459</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>2019</v>
@@ -2922,11 +2939,11 @@
       <c r="D31" s="0" t="n">
         <v>402</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="0" t="n">
         <v>402</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>39.80676329</v>
@@ -2946,10 +2963,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>2019</v>
@@ -2957,11 +2974,11 @@
       <c r="D32" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="0" t="n">
         <v>171</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>49.79986197</v>
@@ -2981,10 +2998,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>2019</v>
@@ -2992,22 +3009,22 @@
       <c r="D33" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="E33" s="0" t="n">
         <v>200</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G33" s="0" t="n">
         <v>28.9488188976378</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>2019</v>
@@ -3015,11 +3032,11 @@
       <c r="D34" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="0" t="n">
         <v>200</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>82.99516908</v>
@@ -3039,10 +3056,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>2019</v>
@@ -3050,22 +3067,22 @@
       <c r="D35" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="E35" s="0" t="n">
         <v>100</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G35" s="0" t="n">
         <v>25.2390243902439</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>2019</v>
@@ -3073,11 +3090,11 @@
       <c r="D36" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="0" t="n">
         <v>300</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>107.1438958</v>
@@ -3097,10 +3114,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>2019</v>
@@ -3108,22 +3125,22 @@
       <c r="D37" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="0" t="n">
         <v>300</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G37" s="0" t="n">
         <v>23.4532374100719</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>2019</v>
@@ -3131,11 +3148,11 @@
       <c r="D38" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="0" t="n">
         <v>100</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>113.0123138</v>
@@ -3155,10 +3172,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>2019</v>
@@ -3166,22 +3183,22 @@
       <c r="D39" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="0" t="n">
         <v>100</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G39" s="0" t="n">
         <v>11.0821467688938</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>2019</v>
@@ -3189,22 +3206,22 @@
       <c r="D40" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="E40" s="1" t="n">
+      <c r="E40" s="0" t="n">
         <v>300</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G40" s="0" t="n">
         <v>34.1347517730496</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>2019</v>
@@ -3212,11 +3229,11 @@
       <c r="D41" s="0" t="n">
         <v>490</v>
       </c>
-      <c r="E41" s="1" t="n">
+      <c r="E41" s="0" t="n">
         <v>490</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>7.636546026</v>
@@ -3236,10 +3253,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>2019</v>
@@ -3247,22 +3264,22 @@
       <c r="D42" s="0" t="n">
         <v>390</v>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="0" t="n">
         <v>390</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G42" s="0" t="n">
         <v>20.82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>2019</v>
@@ -3270,11 +3287,11 @@
       <c r="D43" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="0" t="n">
         <v>90</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G43" s="0" t="n">
         <v>80.48056313</v>
@@ -3294,10 +3311,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>2019</v>
@@ -3305,22 +3322,22 @@
       <c r="D44" s="0" t="n">
         <v>490</v>
       </c>
-      <c r="E44" s="1" t="n">
+      <c r="E44" s="0" t="n">
         <v>490</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G44" s="0" t="n">
         <v>38.5986842105263</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>2019</v>
@@ -3328,22 +3345,22 @@
       <c r="D45" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="E45" s="1" t="n">
+      <c r="E45" s="0" t="n">
         <v>90</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G45" s="0" t="n">
         <v>21.2470308788599</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>2019</v>
@@ -3351,11 +3368,11 @@
       <c r="D46" s="0" t="n">
         <v>520</v>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="E46" s="0" t="n">
         <v>520</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>90.16563147</v>
@@ -3375,10 +3392,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>2019</v>
@@ -3386,22 +3403,22 @@
       <c r="D47" s="0" t="n">
         <v>520</v>
       </c>
-      <c r="E47" s="1" t="n">
+      <c r="E47" s="0" t="n">
         <v>520</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G47" s="0" t="n">
         <v>18.495867768595</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>2019</v>
@@ -3409,11 +3426,11 @@
       <c r="D48" s="0" t="n">
         <v>278</v>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="E48" s="0" t="n">
         <v>278</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>53.0177949</v>
@@ -3433,10 +3450,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>2019</v>
@@ -3444,11 +3461,11 @@
       <c r="D49" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="E49" s="1" t="n">
+      <c r="E49" s="0" t="n">
         <v>107</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>64.2526999</v>
@@ -3468,10 +3485,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>2019</v>
@@ -3479,22 +3496,22 @@
       <c r="D50" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="E50" s="1" t="n">
+      <c r="E50" s="0" t="n">
         <v>107</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G50" s="0" t="n">
         <v>13.1277997364954</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>2019</v>
@@ -3502,34 +3519,34 @@
       <c r="D51" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="E51" s="1" t="n">
+      <c r="E51" s="0" t="n">
         <v>107</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G51" s="0" t="n">
         <v>23.8048780487805</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3554,7 +3571,7 @@
       <selection pane="topLeft" activeCell="S39" activeCellId="0" sqref="S39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>
@@ -3566,18 +3583,18 @@
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>102</v>
@@ -3592,7 +3609,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>130</v>
@@ -3607,7 +3624,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>170</v>
@@ -3622,7 +3639,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>300</v>
@@ -3637,7 +3654,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>370</v>
@@ -3652,7 +3669,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>570</v>
@@ -3667,7 +3684,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>700</v>
@@ -3682,7 +3699,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>770</v>
@@ -3697,7 +3714,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>965</v>
@@ -3715,18 +3732,18 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>90</v>
@@ -3741,7 +3758,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>100</v>
@@ -3756,7 +3773,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>107</v>
@@ -3771,7 +3788,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>171</v>
@@ -3786,7 +3803,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>173</v>
@@ -3801,7 +3818,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>200</v>
@@ -3816,7 +3833,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>278</v>
@@ -3831,7 +3848,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>300</v>
@@ -3846,7 +3863,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>402</v>
@@ -3861,7 +3878,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>490</v>
@@ -3876,7 +3893,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>520</v>
@@ -3891,7 +3908,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>965</v>

</xml_diff>

<commit_message>
added year and month notations to 43 and 44 flux fig components
</commit_message>
<xml_diff>
--- a/data/flux/2019-fluxes.xlsx
+++ b/data/flux/2019-fluxes.xlsx
@@ -426,7 +426,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -609,11 +609,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="32887941"/>
-        <c:axId val="63272554"/>
+        <c:axId val="35688326"/>
+        <c:axId val="78588239"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32887941"/>
+        <c:axId val="35688326"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,12 +669,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63272554"/>
+        <c:crossAx val="78588239"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63272554"/>
+        <c:axId val="78588239"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -739,7 +739,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32887941"/>
+        <c:crossAx val="35688326"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -787,7 +787,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -988,11 +988,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="29278975"/>
-        <c:axId val="46560285"/>
+        <c:axId val="10875065"/>
+        <c:axId val="73486803"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29278975"/>
+        <c:axId val="10875065"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1048,12 +1048,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46560285"/>
+        <c:crossAx val="73486803"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46560285"/>
+        <c:axId val="73486803"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1118,7 +1118,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29278975"/>
+        <c:crossAx val="10875065"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1166,7 +1166,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1382,11 +1382,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="11703092"/>
-        <c:axId val="31850033"/>
+        <c:axId val="53237660"/>
+        <c:axId val="69140891"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="11703092"/>
+        <c:axId val="53237660"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,12 +1442,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31850033"/>
+        <c:crossAx val="69140891"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31850033"/>
+        <c:axId val="69140891"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1512,7 +1512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11703092"/>
+        <c:crossAx val="53237660"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1560,7 +1560,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1761,11 +1761,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="13217630"/>
-        <c:axId val="80376665"/>
+        <c:axId val="25603727"/>
+        <c:axId val="23625191"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13217630"/>
+        <c:axId val="25603727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,12 +1821,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80376665"/>
+        <c:crossAx val="23625191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80376665"/>
+        <c:axId val="23625191"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1891,7 +1891,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13217630"/>
+        <c:crossAx val="25603727"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1950,9 +1950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>401400</xdr:colOff>
+      <xdr:colOff>401040</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1960,8 +1960,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4469040" y="47880"/>
-        <a:ext cx="5144040" cy="4282200"/>
+        <a:off x="4472640" y="47880"/>
+        <a:ext cx="5151600" cy="4281840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1980,9 +1980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>185400</xdr:colOff>
+      <xdr:colOff>185040</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1990,8 +1990,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4382280" y="4513320"/>
-        <a:ext cx="5014800" cy="5219640"/>
+        <a:off x="4385880" y="4513320"/>
+        <a:ext cx="5022360" cy="5219280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2010,9 +2010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>47160</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2020,8 +2020,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9718920" y="28800"/>
-        <a:ext cx="4447440" cy="4512240"/>
+        <a:off x="9730440" y="28800"/>
+        <a:ext cx="4454280" cy="4511880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2040,9 +2040,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>411120</xdr:colOff>
+      <xdr:colOff>410760</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2050,8 +2050,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9515160" y="4513320"/>
-        <a:ext cx="5015160" cy="5219640"/>
+        <a:off x="9526680" y="4513320"/>
+        <a:ext cx="5022000" cy="5219280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2072,10 +2072,10 @@
   <dimension ref="A1:O107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+      <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1014" style="0" width="11.52"/>
   </cols>
@@ -3571,7 +3571,7 @@
       <selection pane="topLeft" activeCell="S39" activeCellId="0" sqref="S39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>

</xml_diff>

<commit_message>
made new nb to proccess only the top collector for cn and d13c
</commit_message>
<xml_diff>
--- a/data/flux/2019-fluxes.xlsx
+++ b/data/flux/2019-fluxes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="85">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">Trap type</t>
   </si>
   <si>
+    <t xml:space="preserve">Chamber</t>
+  </si>
+  <si>
     <t xml:space="preserve">Flux (mg/m2/day)</t>
   </si>
   <si>
@@ -63,10 +66,10 @@
     <t xml:space="preserve">N production rate (nM N/day)</t>
   </si>
   <si>
-    <t xml:space="preserve">d15N vs Air N2 (permil)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d13C vs VPDB (permil)</t>
+    <t xml:space="preserve">d15N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d13C</t>
   </si>
   <si>
     <t xml:space="preserve">1-58_170m_NO2_ctl</t>
@@ -78,9 +81,15 @@
     <t xml:space="preserve">Hybrid</t>
   </si>
   <si>
+    <t xml:space="preserve">control</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-58_170m_NO2_+P</t>
   </si>
   <si>
+    <t xml:space="preserve">particles</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-58_570m_NO2_ctl</t>
   </si>
   <si>
@@ -90,6 +99,9 @@
     <t xml:space="preserve">1-58_570m_NO2_top</t>
   </si>
   <si>
+    <t xml:space="preserve">top</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-58_370m_ctl</t>
   </si>
   <si>
@@ -120,6 +132,9 @@
     <t xml:space="preserve">1-58_770m_net_nw</t>
   </si>
   <si>
+    <t xml:space="preserve">netwash</t>
+  </si>
+  <si>
     <t xml:space="preserve">4-59_130m_NO2_+P</t>
   </si>
   <si>
@@ -163,6 +178,9 @@
   </si>
   <si>
     <t xml:space="preserve">4-52_965m_top/+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combined</t>
   </si>
   <si>
     <t xml:space="preserve">3-54_402m_ctl</t>
@@ -433,7 +451,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -616,11 +634,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99480798"/>
-        <c:axId val="8041198"/>
+        <c:axId val="84922182"/>
+        <c:axId val="91385698"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99480798"/>
+        <c:axId val="84922182"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,12 +694,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8041198"/>
+        <c:crossAx val="91385698"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8041198"/>
+        <c:axId val="91385698"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -746,7 +764,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99480798"/>
+        <c:crossAx val="84922182"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -794,7 +812,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -995,11 +1013,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="3117563"/>
-        <c:axId val="49891212"/>
+        <c:axId val="30949206"/>
+        <c:axId val="39717120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3117563"/>
+        <c:axId val="30949206"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,12 +1073,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49891212"/>
+        <c:crossAx val="39717120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49891212"/>
+        <c:axId val="39717120"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1125,7 +1143,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3117563"/>
+        <c:crossAx val="30949206"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1173,7 +1191,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1389,11 +1407,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="27205375"/>
-        <c:axId val="63422137"/>
+        <c:axId val="85522314"/>
+        <c:axId val="65104200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27205375"/>
+        <c:axId val="85522314"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,12 +1467,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63422137"/>
+        <c:crossAx val="65104200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63422137"/>
+        <c:axId val="65104200"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1519,7 +1537,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27205375"/>
+        <c:crossAx val="85522314"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1567,7 +1585,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1768,11 +1786,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="12689633"/>
-        <c:axId val="41801619"/>
+        <c:axId val="69879890"/>
+        <c:axId val="44319455"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="12689633"/>
+        <c:axId val="69879890"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,12 +1846,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41801619"/>
+        <c:crossAx val="44319455"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41801619"/>
+        <c:axId val="44319455"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1898,7 +1916,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12689633"/>
+        <c:crossAx val="69879890"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1946,7 +1964,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2163,11 +2181,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="15892164"/>
-        <c:axId val="52055203"/>
+        <c:axId val="22949194"/>
+        <c:axId val="61679805"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15892164"/>
+        <c:axId val="22949194"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2223,12 +2241,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52055203"/>
+        <c:crossAx val="61679805"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52055203"/>
+        <c:axId val="61679805"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2284,7 +2302,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15892164"/>
+        <c:crossAx val="22949194"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2311,7 +2329,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2537,11 +2555,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52518917"/>
-        <c:axId val="20854994"/>
+        <c:axId val="92772318"/>
+        <c:axId val="92871"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52518917"/>
+        <c:axId val="92772318"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2597,12 +2615,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20854994"/>
+        <c:crossAx val="92871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20854994"/>
+        <c:axId val="92871"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2658,7 +2676,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52518917"/>
+        <c:crossAx val="92772318"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2696,9 +2714,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>400320</xdr:colOff>
+      <xdr:colOff>399960</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>102600</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2706,8 +2724,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4480560" y="47880"/>
-        <a:ext cx="5165640" cy="4281120"/>
+        <a:off x="4482360" y="47880"/>
+        <a:ext cx="5169600" cy="4280760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2726,9 +2744,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>184320</xdr:colOff>
+      <xdr:colOff>183960</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2736,8 +2754,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4393800" y="4513320"/>
-        <a:ext cx="5036400" cy="5218560"/>
+        <a:off x="4395600" y="4513320"/>
+        <a:ext cx="5040360" cy="5218560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2756,9 +2774,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2766,8 +2784,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9753120" y="28800"/>
-        <a:ext cx="4469040" cy="4511160"/>
+        <a:off x="9759240" y="28800"/>
+        <a:ext cx="4472280" cy="4510800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2786,9 +2804,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>410040</xdr:colOff>
+      <xdr:colOff>409680</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2796,8 +2814,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9549360" y="4513320"/>
-        <a:ext cx="5036760" cy="5218560"/>
+        <a:off x="9555480" y="4513320"/>
+        <a:ext cx="5040000" cy="5218560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2821,9 +2839,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>367920</xdr:colOff>
+      <xdr:colOff>367560</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2831,8 +2849,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12748320" y="4159440"/>
-        <a:ext cx="3062520" cy="3987000"/>
+        <a:off x="12748680" y="4159800"/>
+        <a:ext cx="3062160" cy="3986640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2851,9 +2869,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>555120</xdr:colOff>
+      <xdr:colOff>554760</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2861,8 +2879,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9684360" y="4159440"/>
-        <a:ext cx="3062520" cy="3987000"/>
+        <a:off x="9684720" y="4159800"/>
+        <a:ext cx="3062160" cy="3986640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2880,19 +2898,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O107"/>
+  <dimension ref="A1:P107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1:O1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="1" style="1" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1014" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1015" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2932,19 +2951,22 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2019</v>
@@ -2956,18 +2978,21 @@
         <v>170</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>7.75319567354966</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2019</v>
@@ -2979,27 +3004,30 @@
         <v>170</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>14.62984724</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>100.3934843</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="K3" s="1" t="n">
         <v>202.5483083</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="L3" s="1" t="n">
         <v>2.017544363</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2019</v>
@@ -3011,18 +3039,21 @@
         <v>570</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>3.6622641509434</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2019</v>
@@ -3034,30 +3065,33 @@
         <v>570</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>41.66411217</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>7.29879518072289</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="J5" s="1" t="n">
         <v>15.92666572</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="K5" s="1" t="n">
         <v>52.53922915</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>3.298821617</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2019</v>
@@ -3069,18 +3103,21 @@
         <v>570</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>9.72617743702081</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2019</v>
@@ -3092,18 +3129,21 @@
         <v>370</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>1.85815047021944</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>2019</v>
@@ -3115,30 +3155,33 @@
         <v>370</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>19.66438915</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="I8" s="1" t="n">
         <v>5.4967585089141</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="J8" s="1" t="n">
         <v>14.76380988</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="K8" s="1" t="n">
         <v>14.70959842</v>
       </c>
-      <c r="K8" s="1" t="n">
+      <c r="L8" s="1" t="n">
         <v>0.9963280845</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>2019</v>
@@ -3150,18 +3193,21 @@
         <v>370</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>6.57961447055717</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>2019</v>
@@ -3173,18 +3219,21 @@
         <v>102</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>24.9704142011834</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>2019</v>
@@ -3196,30 +3245,33 @@
         <v>102</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>31.44875954</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="I11" s="1" t="n">
         <v>5.73174108688127</v>
       </c>
-      <c r="I11" s="1" t="n">
+      <c r="J11" s="1" t="n">
         <v>38.90881844</v>
       </c>
-      <c r="J11" s="1" t="n">
+      <c r="K11" s="1" t="n">
         <v>120.2948594</v>
       </c>
-      <c r="K11" s="1" t="n">
+      <c r="L11" s="1" t="n">
         <v>3.091711962</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>2019</v>
@@ -3231,18 +3283,21 @@
         <v>102</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>9.5391061452514</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>2019</v>
@@ -3254,30 +3309,33 @@
         <v>770</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>20.11954101</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="I13" s="1" t="n">
         <v>8.39540816326531</v>
       </c>
-      <c r="I13" s="1" t="n">
+      <c r="J13" s="1" t="n">
         <v>18.77829274</v>
       </c>
-      <c r="J13" s="1" t="n">
+      <c r="K13" s="1" t="n">
         <v>41.23605442</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="L13" s="1" t="n">
         <v>2.195942677</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>2019</v>
@@ -3289,18 +3347,21 @@
         <v>770</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>11.0183881064163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>2019</v>
@@ -3312,18 +3373,21 @@
         <v>770</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>7.13300230537329</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>2019</v>
@@ -3335,27 +3399,30 @@
         <v>130</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>54.59667624</v>
       </c>
-      <c r="I16" s="1" t="n">
+      <c r="J16" s="1" t="n">
         <v>36.64505423</v>
       </c>
-      <c r="J16" s="1" t="n">
+      <c r="K16" s="1" t="n">
         <v>83.36974729</v>
       </c>
-      <c r="K16" s="1" t="n">
+      <c r="L16" s="1" t="n">
         <v>2.27506137</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>2019</v>
@@ -3367,18 +3434,21 @@
         <v>130</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>10.0321931589537</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>2019</v>
@@ -3390,18 +3460,21 @@
         <v>130</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>25.396694214876</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>2019</v>
@@ -3413,30 +3486,33 @@
         <v>300</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="1" t="n">
         <v>82.77252678</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="I19" s="1" t="n">
         <v>8.90150250417362</v>
       </c>
-      <c r="I19" s="1" t="n">
+      <c r="J19" s="1" t="n">
         <v>25.61694486</v>
       </c>
-      <c r="J19" s="1" t="n">
+      <c r="K19" s="1" t="n">
         <v>43.50938879</v>
       </c>
-      <c r="K19" s="1" t="n">
+      <c r="L19" s="1" t="n">
         <v>1.698461273</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>2019</v>
@@ -3448,30 +3524,33 @@
         <v>700</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>61.24302838</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="I20" s="1" t="n">
         <v>10.3601496725912</v>
       </c>
-      <c r="I20" s="1" t="n">
+      <c r="J20" s="1" t="n">
         <v>29.98676977</v>
       </c>
-      <c r="J20" s="1" t="n">
+      <c r="K20" s="1" t="n">
         <v>86.57859897</v>
       </c>
-      <c r="K20" s="1" t="n">
+      <c r="L20" s="1" t="n">
         <v>2.887226589</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>2019</v>
@@ -3483,18 +3562,21 @@
         <v>700</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>11.1135940409683</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>2019</v>
@@ -3506,18 +3588,21 @@
         <v>700</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>12.3389830508475</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>2019</v>
@@ -3529,27 +3614,30 @@
         <v>965</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>51.08955421</v>
       </c>
-      <c r="I23" s="1" t="n">
+      <c r="J23" s="1" t="n">
         <v>16.79816516</v>
       </c>
-      <c r="J23" s="1" t="n">
+      <c r="K23" s="1" t="n">
         <v>69.3490879</v>
       </c>
-      <c r="K23" s="1" t="n">
+      <c r="L23" s="1" t="n">
         <v>7.700191459</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>2019</v>
@@ -3561,18 +3649,21 @@
         <v>965</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>12.3266761768902</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>2019</v>
@@ -3584,18 +3675,21 @@
         <v>965</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>35.8697318007663</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>2019</v>
@@ -3607,27 +3701,30 @@
         <v>173</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>53.1000796</v>
       </c>
-      <c r="I26" s="1" t="n">
+      <c r="J26" s="1" t="n">
         <v>30.541058</v>
       </c>
-      <c r="J26" s="1" t="n">
+      <c r="K26" s="1" t="n">
         <v>154.782931</v>
       </c>
-      <c r="K26" s="1" t="n">
+      <c r="L26" s="1" t="n">
         <v>5.0680278</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>2019</v>
@@ -3639,18 +3736,21 @@
         <v>173</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>29.8271604938272</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2019</v>
@@ -3662,18 +3762,21 @@
         <v>173</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>14.1515151515152</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2019</v>
@@ -3685,30 +3788,33 @@
         <v>965</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>21.16318464</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="I29" s="1" t="n">
         <v>11.2737520128825</v>
       </c>
-      <c r="I29" s="1" t="n">
+      <c r="J29" s="1" t="n">
         <v>18.53206428</v>
       </c>
-      <c r="J29" s="1" t="n">
+      <c r="K29" s="1" t="n">
         <v>186.4108454</v>
       </c>
-      <c r="K29" s="1" t="n">
+      <c r="L29" s="1" t="n">
         <v>10.05882791</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>2019</v>
@@ -3720,18 +3826,21 @@
         <v>402</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>30.1541353383459</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>2019</v>
@@ -3743,27 +3852,30 @@
         <v>402</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>39.80676329</v>
       </c>
-      <c r="I31" s="1" t="n">
+      <c r="J31" s="1" t="n">
         <v>34.43275128</v>
       </c>
-      <c r="J31" s="1" t="n">
+      <c r="K31" s="1" t="n">
         <v>398.5595814</v>
       </c>
-      <c r="K31" s="1" t="n">
+      <c r="L31" s="1" t="n">
         <v>11.57501409</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>2019</v>
@@ -3775,27 +3887,30 @@
         <v>171</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>49.79986197</v>
       </c>
-      <c r="I32" s="1" t="n">
+      <c r="J32" s="1" t="n">
         <v>45.06542609</v>
       </c>
-      <c r="J32" s="1" t="n">
+      <c r="K32" s="1" t="n">
         <v>96.27078959</v>
       </c>
-      <c r="K32" s="1" t="n">
+      <c r="L32" s="1" t="n">
         <v>2.136244965</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>2019</v>
@@ -3807,18 +3922,21 @@
         <v>200</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>28.9488188976378</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>2019</v>
@@ -3830,30 +3948,33 @@
         <v>200</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>82.99516908</v>
       </c>
-      <c r="H34" s="1" t="n">
+      <c r="I34" s="1" t="n">
         <v>10.7176470588235</v>
       </c>
-      <c r="I34" s="1" t="n">
+      <c r="J34" s="1" t="n">
         <v>22.29103516</v>
       </c>
-      <c r="J34" s="1" t="n">
+      <c r="K34" s="1" t="n">
         <v>187.1856453</v>
       </c>
-      <c r="K34" s="1" t="n">
+      <c r="L34" s="1" t="n">
         <v>8.397350951</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>2019</v>
@@ -3865,18 +3986,21 @@
         <v>100</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>25.2390243902439</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>2019</v>
@@ -3888,27 +4012,30 @@
         <v>300</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>107.1438958</v>
       </c>
-      <c r="I36" s="1" t="n">
+      <c r="J36" s="1" t="n">
         <v>21.5044534</v>
       </c>
-      <c r="J36" s="1" t="n">
+      <c r="K36" s="1" t="n">
         <v>363.0646116</v>
       </c>
-      <c r="K36" s="1" t="n">
+      <c r="L36" s="1" t="n">
         <v>16.88322902</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>2019</v>
@@ -3920,18 +4047,21 @@
         <v>300</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="1" t="n">
         <v>23.4532374100719</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>2019</v>
@@ -3943,27 +4073,30 @@
         <v>100</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="1" t="n">
         <v>113.0123138</v>
       </c>
-      <c r="I38" s="1" t="n">
+      <c r="J38" s="1" t="n">
         <v>24.79294243</v>
       </c>
-      <c r="J38" s="1" t="n">
+      <c r="K38" s="1" t="n">
         <v>451.5821744</v>
       </c>
-      <c r="K38" s="1" t="n">
+      <c r="L38" s="1" t="n">
         <v>18.21414201</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>2019</v>
@@ -3975,18 +4108,21 @@
         <v>100</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="1" t="n">
         <v>11.0821467688938</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>2019</v>
@@ -3998,18 +4134,21 @@
         <v>300</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="1" t="n">
         <v>34.1347517730496</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>2019</v>
@@ -4021,27 +4160,30 @@
         <v>490</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" s="1" t="n">
         <v>7.636546026</v>
       </c>
-      <c r="I41" s="1" t="n">
+      <c r="J41" s="1" t="n">
         <v>20.67419312</v>
       </c>
-      <c r="J41" s="1" t="n">
+      <c r="K41" s="1" t="n">
         <v>245.6279172</v>
       </c>
-      <c r="K41" s="1" t="n">
+      <c r="L41" s="1" t="n">
         <v>11.88089498</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>2019</v>
@@ -4053,18 +4195,21 @@
         <v>390</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="1" t="n">
         <v>20.82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>2019</v>
@@ -4076,30 +4221,33 @@
         <v>90</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G43" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="1" t="n">
         <v>80.48056313</v>
       </c>
-      <c r="H43" s="1" t="n">
+      <c r="I43" s="1" t="n">
         <v>4.62063615205586</v>
       </c>
-      <c r="I43" s="1" t="n">
+      <c r="J43" s="1" t="n">
         <v>353.5566298</v>
       </c>
-      <c r="J43" s="1" t="n">
+      <c r="K43" s="1" t="n">
         <v>1558.049231</v>
       </c>
-      <c r="K43" s="1" t="n">
+      <c r="L43" s="1" t="n">
         <v>4.406788334</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>2019</v>
@@ -4111,18 +4259,21 @@
         <v>490</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G44" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="1" t="n">
         <v>38.5986842105263</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>2019</v>
@@ -4134,18 +4285,21 @@
         <v>90</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G45" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="1" t="n">
         <v>21.2470308788599</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>2019</v>
@@ -4157,27 +4311,30 @@
         <v>520</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G46" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="1" t="n">
         <v>90.16563147</v>
       </c>
-      <c r="I46" s="1" t="n">
+      <c r="J46" s="1" t="n">
         <v>86.81522804</v>
       </c>
-      <c r="J46" s="1" t="n">
+      <c r="K46" s="1" t="n">
         <v>332.7506362</v>
       </c>
-      <c r="K46" s="1" t="n">
+      <c r="L46" s="1" t="n">
         <v>3.832860245</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>2019</v>
@@ -4189,18 +4346,21 @@
         <v>520</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="1" t="n">
         <v>18.495867768595</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>2019</v>
@@ -4212,30 +4372,33 @@
         <v>278</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G48" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" s="1" t="n">
         <v>53.0177949</v>
       </c>
-      <c r="H48" s="1" t="n">
+      <c r="I48" s="1" t="n">
         <v>13.5171898355755</v>
       </c>
-      <c r="I48" s="1" t="n">
+      <c r="J48" s="1" t="n">
         <v>52.99719101</v>
       </c>
-      <c r="J48" s="1" t="n">
+      <c r="K48" s="1" t="n">
         <v>204.4910401</v>
       </c>
-      <c r="K48" s="1" t="n">
+      <c r="L48" s="1" t="n">
         <v>3.858526013</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>2019</v>
@@ -4247,30 +4410,33 @@
         <v>107</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G49" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="1" t="n">
         <v>64.2526999</v>
       </c>
-      <c r="H49" s="1" t="n">
+      <c r="I49" s="1" t="n">
         <v>11.9092872570194</v>
       </c>
-      <c r="I49" s="1" t="n">
+      <c r="J49" s="1" t="n">
         <v>16.55766079</v>
       </c>
-      <c r="J49" s="1" t="n">
+      <c r="K49" s="1" t="n">
         <v>272.0780859</v>
       </c>
-      <c r="K49" s="1" t="n">
+      <c r="L49" s="1" t="n">
         <v>16.43215725</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>2019</v>
@@ -4282,18 +4448,21 @@
         <v>107</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G50" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H50" s="1" t="n">
         <v>13.1277997364954</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>2019</v>
@@ -4305,30 +4474,33 @@
         <v>107</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G51" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51" s="1" t="n">
         <v>23.8048780487805</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4350,10 +4522,10 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S39" activeCellId="1" sqref="N1:O1 S39"/>
+      <selection pane="topLeft" activeCell="S39" activeCellId="0" sqref="S39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>
@@ -4365,18 +4537,18 @@
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>102</v>
@@ -4391,7 +4563,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>130</v>
@@ -4406,7 +4578,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>170</v>
@@ -4421,7 +4593,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>300</v>
@@ -4436,7 +4608,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>370</v>
@@ -4451,7 +4623,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>570</v>
@@ -4466,7 +4638,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>700</v>
@@ -4481,7 +4653,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>770</v>
@@ -4496,7 +4668,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>965</v>
@@ -4514,18 +4686,18 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>90</v>
@@ -4540,7 +4712,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>100</v>
@@ -4555,7 +4727,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>107</v>
@@ -4570,7 +4742,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>171</v>
@@ -4585,7 +4757,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>173</v>
@@ -4600,7 +4772,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>200</v>
@@ -4615,7 +4787,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>278</v>
@@ -4630,7 +4802,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>300</v>
@@ -4645,7 +4817,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>402</v>
@@ -4660,7 +4832,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>490</v>
@@ -4675,7 +4847,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>520</v>
@@ -4690,7 +4862,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>965</v>
@@ -4723,7 +4895,7 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L47" activeCellId="1" sqref="N1:O1 L47"/>
+      <selection pane="topLeft" activeCell="L47" activeCellId="0" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4748,18 +4920,18 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>170</v>
@@ -4768,15 +4940,15 @@
         <v>170</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>170</v>
@@ -4785,7 +4957,7 @@
         <v>170</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>202.5483083</v>
@@ -4797,10 +4969,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>570</v>
@@ -4809,15 +4981,15 @@
         <v>570</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>570</v>
@@ -4826,7 +4998,7 @@
         <v>570</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>52.53922915</v>
@@ -4838,10 +5010,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>570</v>
@@ -4850,15 +5022,15 @@
         <v>570</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>370</v>
@@ -4867,15 +5039,15 @@
         <v>370</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>370</v>
@@ -4884,7 +5056,7 @@
         <v>370</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>14.70959842</v>
@@ -4896,10 +5068,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>370</v>
@@ -4908,15 +5080,15 @@
         <v>370</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>102</v>
@@ -4925,15 +5097,15 @@
         <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>102</v>
@@ -4942,7 +5114,7 @@
         <v>102</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>120.2948594</v>
@@ -4954,10 +5126,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>102</v>
@@ -4966,15 +5138,15 @@
         <v>102</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>770</v>
@@ -4983,7 +5155,7 @@
         <v>770</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>41.23605442</v>
@@ -4995,10 +5167,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>770</v>
@@ -5007,15 +5179,15 @@
         <v>770</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>770</v>
@@ -5024,15 +5196,15 @@
         <v>770</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>130</v>
@@ -5041,7 +5213,7 @@
         <v>130</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>83.36974729</v>
@@ -5053,10 +5225,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>130</v>
@@ -5065,15 +5237,15 @@
         <v>130</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>130</v>
@@ -5082,15 +5254,15 @@
         <v>130</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>300</v>
@@ -5099,7 +5271,7 @@
         <v>300</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>43.50938879</v>
@@ -5111,10 +5283,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>700</v>
@@ -5123,7 +5295,7 @@
         <v>700</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>86.57859897</v>
@@ -5135,10 +5307,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>700</v>
@@ -5147,15 +5319,15 @@
         <v>700</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>700</v>
@@ -5164,15 +5336,15 @@
         <v>700</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>965</v>
@@ -5181,7 +5353,7 @@
         <v>965</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>69.3490879</v>
@@ -5193,10 +5365,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>965</v>
@@ -5205,15 +5377,15 @@
         <v>965</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>965</v>
@@ -5222,7 +5394,7 @@
         <v>965</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5242,18 +5414,18 @@
         <v>5</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>173</v>
@@ -5262,7 +5434,7 @@
         <v>173</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>154.782931</v>
@@ -5274,10 +5446,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>173</v>
@@ -5286,15 +5458,15 @@
         <v>173</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>173</v>
@@ -5303,15 +5475,15 @@
         <v>173</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>965</v>
@@ -5320,7 +5492,7 @@
         <v>965</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>186.4108454</v>
@@ -5332,10 +5504,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>402</v>
@@ -5344,15 +5516,15 @@
         <v>402</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>402</v>
@@ -5361,7 +5533,7 @@
         <v>402</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>398.5595814</v>
@@ -5373,10 +5545,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>171</v>
@@ -5385,7 +5557,7 @@
         <v>171</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>96.27078959</v>
@@ -5397,10 +5569,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>200</v>
@@ -5409,15 +5581,15 @@
         <v>200</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>200</v>
@@ -5426,7 +5598,7 @@
         <v>200</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>187.1856453</v>
@@ -5438,10 +5610,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>100</v>
@@ -5450,15 +5622,15 @@
         <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>300</v>
@@ -5467,7 +5639,7 @@
         <v>300</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37" s="1" t="n">
         <v>363.0646116</v>
@@ -5479,10 +5651,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>300</v>
@@ -5491,15 +5663,15 @@
         <v>300</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>100</v>
@@ -5508,7 +5680,7 @@
         <v>100</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F39" s="1" t="n">
         <v>451.5821744</v>
@@ -5520,10 +5692,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>100</v>
@@ -5532,15 +5704,15 @@
         <v>100</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>300</v>
@@ -5549,15 +5721,15 @@
         <v>300</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>490</v>
@@ -5566,7 +5738,7 @@
         <v>490</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>245.6279172</v>
@@ -5578,10 +5750,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>390</v>
@@ -5590,15 +5762,15 @@
         <v>390</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>90</v>
@@ -5607,7 +5779,7 @@
         <v>90</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>1558.049231</v>
@@ -5619,10 +5791,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>490</v>
@@ -5631,15 +5803,15 @@
         <v>490</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>90</v>
@@ -5648,15 +5820,15 @@
         <v>90</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>520</v>
@@ -5665,7 +5837,7 @@
         <v>520</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>332.7506362</v>
@@ -5677,10 +5849,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>520</v>
@@ -5689,15 +5861,15 @@
         <v>520</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>278</v>
@@ -5706,7 +5878,7 @@
         <v>278</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F49" s="1" t="n">
         <v>204.4910401</v>
@@ -5718,10 +5890,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>107</v>
@@ -5730,7 +5902,7 @@
         <v>107</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F50" s="1" t="n">
         <v>272.0780859</v>
@@ -5742,10 +5914,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>107</v>
@@ -5754,15 +5926,15 @@
         <v>107</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>107</v>
@@ -5771,27 +5943,27 @@
         <v>107</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added inc data to 2019 fluxes
</commit_message>
<xml_diff>
--- a/data/flux/2019-fluxes.xlsx
+++ b/data/flux/2019-fluxes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="89">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">Chamber</t>
   </si>
   <si>
+    <t xml:space="preserve">Incubation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Flux (mg/m2/day)</t>
   </si>
   <si>
@@ -84,6 +87,9 @@
     <t xml:space="preserve">control</t>
   </si>
   <si>
+    <t xml:space="preserve">NO2</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-58_170m_NO2_+P</t>
   </si>
   <si>
@@ -105,6 +111,9 @@
     <t xml:space="preserve">1-58_370m_ctl</t>
   </si>
   <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-58_370m_+P</t>
   </si>
   <si>
@@ -145,6 +154,9 @@
   </si>
   <si>
     <t xml:space="preserve">4-59_300m_Fe_top_split</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe</t>
   </si>
   <si>
     <t xml:space="preserve">4-59_700m_NO2_+P</t>
@@ -451,7 +463,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -634,11 +646,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="84922182"/>
-        <c:axId val="91385698"/>
+        <c:axId val="96207436"/>
+        <c:axId val="76600765"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84922182"/>
+        <c:axId val="96207436"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,12 +706,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91385698"/>
+        <c:crossAx val="76600765"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91385698"/>
+        <c:axId val="76600765"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -764,7 +776,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84922182"/>
+        <c:crossAx val="96207436"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -812,7 +824,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1013,11 +1025,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="30949206"/>
-        <c:axId val="39717120"/>
+        <c:axId val="12901862"/>
+        <c:axId val="93327045"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30949206"/>
+        <c:axId val="12901862"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1073,12 +1085,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39717120"/>
+        <c:crossAx val="93327045"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39717120"/>
+        <c:axId val="93327045"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1143,7 +1155,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30949206"/>
+        <c:crossAx val="12901862"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1191,7 +1203,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1407,11 +1419,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="85522314"/>
-        <c:axId val="65104200"/>
+        <c:axId val="99072178"/>
+        <c:axId val="46759747"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85522314"/>
+        <c:axId val="99072178"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,12 +1479,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65104200"/>
+        <c:crossAx val="46759747"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65104200"/>
+        <c:axId val="46759747"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1537,7 +1549,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85522314"/>
+        <c:crossAx val="99072178"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1585,7 +1597,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1786,11 +1798,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="69879890"/>
-        <c:axId val="44319455"/>
+        <c:axId val="30431186"/>
+        <c:axId val="20768676"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69879890"/>
+        <c:axId val="30431186"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1846,12 +1858,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44319455"/>
+        <c:crossAx val="20768676"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44319455"/>
+        <c:axId val="20768676"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1916,7 +1928,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69879890"/>
+        <c:crossAx val="30431186"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1964,7 +1976,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2181,11 +2193,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="22949194"/>
-        <c:axId val="61679805"/>
+        <c:axId val="77155396"/>
+        <c:axId val="30072250"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="22949194"/>
+        <c:axId val="77155396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,12 +2253,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61679805"/>
+        <c:crossAx val="30072250"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61679805"/>
+        <c:axId val="30072250"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2302,7 +2314,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22949194"/>
+        <c:crossAx val="77155396"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2329,7 +2341,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2555,11 +2567,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="92772318"/>
-        <c:axId val="92871"/>
+        <c:axId val="9467864"/>
+        <c:axId val="57914908"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92772318"/>
+        <c:axId val="9467864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,12 +2627,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92871"/>
+        <c:crossAx val="57914908"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92871"/>
+        <c:axId val="57914908"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2676,7 +2688,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92772318"/>
+        <c:crossAx val="9467864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2714,9 +2726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>399960</xdr:colOff>
+      <xdr:colOff>399600</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>102240</xdr:rowOff>
+      <xdr:rowOff>101880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2724,8 +2736,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4482360" y="47880"/>
-        <a:ext cx="5169600" cy="4280760"/>
+        <a:off x="4486320" y="47880"/>
+        <a:ext cx="5176800" cy="4280400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2744,9 +2756,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>183960</xdr:colOff>
+      <xdr:colOff>183600</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2754,8 +2766,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4395600" y="4513320"/>
-        <a:ext cx="5040360" cy="5218560"/>
+        <a:off x="4399560" y="4513320"/>
+        <a:ext cx="5047560" cy="5218200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2774,9 +2786,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>45360</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2784,8 +2796,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9759240" y="28800"/>
-        <a:ext cx="4472280" cy="4510800"/>
+        <a:off x="9770760" y="28800"/>
+        <a:ext cx="4479480" cy="4510440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2804,9 +2816,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>409680</xdr:colOff>
+      <xdr:colOff>409320</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2814,8 +2826,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9555480" y="4513320"/>
-        <a:ext cx="5040000" cy="5218560"/>
+        <a:off x="9567000" y="4513320"/>
+        <a:ext cx="5047200" cy="5218200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2839,9 +2851,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>367560</xdr:colOff>
+      <xdr:colOff>367200</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2850,7 +2862,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12748680" y="4159800"/>
-        <a:ext cx="3062160" cy="3986640"/>
+        <a:ext cx="3061800" cy="3986280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2869,9 +2881,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>554760</xdr:colOff>
+      <xdr:colOff>554400</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2880,7 +2892,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9684720" y="4159800"/>
-        <a:ext cx="3062160" cy="3986640"/>
+        <a:ext cx="3061800" cy="3986280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2898,17 +2910,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P107"/>
+  <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1015" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2954,19 +2966,22 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2019</v>
@@ -2978,21 +2993,24 @@
         <v>170</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>7.75319567354966</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2019</v>
@@ -3004,30 +3022,33 @@
         <v>170</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>14.62984724</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="K3" s="1" t="n">
         <v>100.3934843</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="L3" s="1" t="n">
         <v>202.5483083</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="M3" s="1" t="n">
         <v>2.017544363</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2019</v>
@@ -3039,21 +3060,24 @@
         <v>570</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <v>3.6622641509434</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2019</v>
@@ -3065,33 +3089,36 @@
         <v>570</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>41.66411217</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="J5" s="1" t="n">
         <v>7.29879518072289</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="K5" s="1" t="n">
         <v>15.92666572</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>52.53922915</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="M5" s="1" t="n">
         <v>3.298821617</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2019</v>
@@ -3103,21 +3130,24 @@
         <v>570</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="n">
         <v>9.72617743702081</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2019</v>
@@ -3129,21 +3159,24 @@
         <v>370</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="n">
         <v>1.85815047021944</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>2019</v>
@@ -3155,33 +3188,36 @@
         <v>370</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <v>19.66438915</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="J8" s="1" t="n">
         <v>5.4967585089141</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="K8" s="1" t="n">
         <v>14.76380988</v>
       </c>
-      <c r="K8" s="1" t="n">
+      <c r="L8" s="1" t="n">
         <v>14.70959842</v>
       </c>
-      <c r="L8" s="1" t="n">
+      <c r="M8" s="1" t="n">
         <v>0.9963280845</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>2019</v>
@@ -3193,21 +3229,24 @@
         <v>370</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="1" t="n">
         <v>6.57961447055717</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>2019</v>
@@ -3219,21 +3258,24 @@
         <v>102</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="1" t="n">
         <v>24.9704142011834</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>2019</v>
@@ -3245,33 +3287,36 @@
         <v>102</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="1" t="n">
         <v>31.44875954</v>
       </c>
-      <c r="I11" s="1" t="n">
+      <c r="J11" s="1" t="n">
         <v>5.73174108688127</v>
       </c>
-      <c r="J11" s="1" t="n">
+      <c r="K11" s="1" t="n">
         <v>38.90881844</v>
       </c>
-      <c r="K11" s="1" t="n">
+      <c r="L11" s="1" t="n">
         <v>120.2948594</v>
       </c>
-      <c r="L11" s="1" t="n">
+      <c r="M11" s="1" t="n">
         <v>3.091711962</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>2019</v>
@@ -3283,21 +3328,24 @@
         <v>102</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="1" t="n">
         <v>9.5391061452514</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>2019</v>
@@ -3309,33 +3357,36 @@
         <v>770</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="1" t="n">
         <v>20.11954101</v>
       </c>
-      <c r="I13" s="1" t="n">
+      <c r="J13" s="1" t="n">
         <v>8.39540816326531</v>
       </c>
-      <c r="J13" s="1" t="n">
+      <c r="K13" s="1" t="n">
         <v>18.77829274</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="L13" s="1" t="n">
         <v>41.23605442</v>
       </c>
-      <c r="L13" s="1" t="n">
+      <c r="M13" s="1" t="n">
         <v>2.195942677</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>2019</v>
@@ -3347,21 +3398,24 @@
         <v>770</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1" t="n">
         <v>11.0183881064163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>2019</v>
@@ -3373,21 +3427,24 @@
         <v>770</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="1" t="n">
         <v>7.13300230537329</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>2019</v>
@@ -3399,30 +3456,33 @@
         <v>130</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="1" t="n">
+      <c r="I16" s="1" t="n">
         <v>54.59667624</v>
       </c>
-      <c r="J16" s="1" t="n">
+      <c r="K16" s="1" t="n">
         <v>36.64505423</v>
       </c>
-      <c r="K16" s="1" t="n">
+      <c r="L16" s="1" t="n">
         <v>83.36974729</v>
       </c>
-      <c r="L16" s="1" t="n">
+      <c r="M16" s="1" t="n">
         <v>2.27506137</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>2019</v>
@@ -3434,21 +3494,24 @@
         <v>130</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="1" t="n">
         <v>10.0321931589537</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>2019</v>
@@ -3460,21 +3523,24 @@
         <v>130</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="1" t="n">
         <v>25.396694214876</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>2019</v>
@@ -3486,33 +3552,36 @@
         <v>300</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="1" t="n">
         <v>82.77252678</v>
       </c>
-      <c r="I19" s="1" t="n">
+      <c r="J19" s="1" t="n">
         <v>8.90150250417362</v>
       </c>
-      <c r="J19" s="1" t="n">
+      <c r="K19" s="1" t="n">
         <v>25.61694486</v>
       </c>
-      <c r="K19" s="1" t="n">
+      <c r="L19" s="1" t="n">
         <v>43.50938879</v>
       </c>
-      <c r="L19" s="1" t="n">
+      <c r="M19" s="1" t="n">
         <v>1.698461273</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>2019</v>
@@ -3524,33 +3593,36 @@
         <v>700</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="I20" s="1" t="n">
         <v>61.24302838</v>
       </c>
-      <c r="I20" s="1" t="n">
+      <c r="J20" s="1" t="n">
         <v>10.3601496725912</v>
       </c>
-      <c r="J20" s="1" t="n">
+      <c r="K20" s="1" t="n">
         <v>29.98676977</v>
       </c>
-      <c r="K20" s="1" t="n">
+      <c r="L20" s="1" t="n">
         <v>86.57859897</v>
       </c>
-      <c r="L20" s="1" t="n">
+      <c r="M20" s="1" t="n">
         <v>2.887226589</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>2019</v>
@@ -3562,21 +3634,24 @@
         <v>700</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="1" t="n">
         <v>11.1135940409683</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>2019</v>
@@ -3588,21 +3663,24 @@
         <v>700</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="1" t="n">
         <v>12.3389830508475</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>2019</v>
@@ -3614,30 +3692,33 @@
         <v>965</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="1" t="n">
         <v>51.08955421</v>
       </c>
-      <c r="J23" s="1" t="n">
+      <c r="K23" s="1" t="n">
         <v>16.79816516</v>
       </c>
-      <c r="K23" s="1" t="n">
+      <c r="L23" s="1" t="n">
         <v>69.3490879</v>
       </c>
-      <c r="L23" s="1" t="n">
+      <c r="M23" s="1" t="n">
         <v>7.700191459</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>2019</v>
@@ -3649,21 +3730,24 @@
         <v>965</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="1" t="n">
         <v>12.3266761768902</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>2019</v>
@@ -3675,21 +3759,24 @@
         <v>965</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="1" t="n">
         <v>35.8697318007663</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>2019</v>
@@ -3701,30 +3788,33 @@
         <v>173</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="1" t="n">
         <v>53.1000796</v>
       </c>
-      <c r="J26" s="1" t="n">
+      <c r="K26" s="1" t="n">
         <v>30.541058</v>
       </c>
-      <c r="K26" s="1" t="n">
+      <c r="L26" s="1" t="n">
         <v>154.782931</v>
       </c>
-      <c r="L26" s="1" t="n">
+      <c r="M26" s="1" t="n">
         <v>5.0680278</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>2019</v>
@@ -3736,21 +3826,24 @@
         <v>173</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="1" t="n">
         <v>29.8271604938272</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2019</v>
@@ -3762,21 +3855,24 @@
         <v>173</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="1" t="n">
         <v>14.1515151515152</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2019</v>
@@ -3788,33 +3884,36 @@
         <v>965</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H29" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="1" t="n">
         <v>21.16318464</v>
       </c>
-      <c r="I29" s="1" t="n">
+      <c r="J29" s="1" t="n">
         <v>11.2737520128825</v>
       </c>
-      <c r="J29" s="1" t="n">
+      <c r="K29" s="1" t="n">
         <v>18.53206428</v>
       </c>
-      <c r="K29" s="1" t="n">
+      <c r="L29" s="1" t="n">
         <v>186.4108454</v>
       </c>
-      <c r="L29" s="1" t="n">
+      <c r="M29" s="1" t="n">
         <v>10.05882791</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>2019</v>
@@ -3826,21 +3925,24 @@
         <v>402</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="1" t="n">
         <v>30.1541353383459</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>2019</v>
@@ -3852,30 +3954,33 @@
         <v>402</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="1" t="n">
         <v>39.80676329</v>
       </c>
-      <c r="J31" s="1" t="n">
+      <c r="K31" s="1" t="n">
         <v>34.43275128</v>
       </c>
-      <c r="K31" s="1" t="n">
+      <c r="L31" s="1" t="n">
         <v>398.5595814</v>
       </c>
-      <c r="L31" s="1" t="n">
+      <c r="M31" s="1" t="n">
         <v>11.57501409</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>2019</v>
@@ -3887,30 +3992,33 @@
         <v>171</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" s="1" t="n">
         <v>49.79986197</v>
       </c>
-      <c r="J32" s="1" t="n">
+      <c r="K32" s="1" t="n">
         <v>45.06542609</v>
       </c>
-      <c r="K32" s="1" t="n">
+      <c r="L32" s="1" t="n">
         <v>96.27078959</v>
       </c>
-      <c r="L32" s="1" t="n">
+      <c r="M32" s="1" t="n">
         <v>2.136244965</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>2019</v>
@@ -3922,21 +4030,24 @@
         <v>200</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="1" t="n">
         <v>28.9488188976378</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>2019</v>
@@ -3948,33 +4059,36 @@
         <v>200</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="1" t="n">
         <v>82.99516908</v>
       </c>
-      <c r="I34" s="1" t="n">
+      <c r="J34" s="1" t="n">
         <v>10.7176470588235</v>
       </c>
-      <c r="J34" s="1" t="n">
+      <c r="K34" s="1" t="n">
         <v>22.29103516</v>
       </c>
-      <c r="K34" s="1" t="n">
+      <c r="L34" s="1" t="n">
         <v>187.1856453</v>
       </c>
-      <c r="L34" s="1" t="n">
+      <c r="M34" s="1" t="n">
         <v>8.397350951</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>2019</v>
@@ -3986,21 +4100,24 @@
         <v>100</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="1" t="n">
         <v>25.2390243902439</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>2019</v>
@@ -4012,30 +4129,33 @@
         <v>300</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="1" t="n">
         <v>107.1438958</v>
       </c>
-      <c r="J36" s="1" t="n">
+      <c r="K36" s="1" t="n">
         <v>21.5044534</v>
       </c>
-      <c r="K36" s="1" t="n">
+      <c r="L36" s="1" t="n">
         <v>363.0646116</v>
       </c>
-      <c r="L36" s="1" t="n">
+      <c r="M36" s="1" t="n">
         <v>16.88322902</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>2019</v>
@@ -4047,21 +4167,24 @@
         <v>300</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="1" t="n">
+      <c r="I37" s="1" t="n">
         <v>23.4532374100719</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>2019</v>
@@ -4073,30 +4196,33 @@
         <v>100</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H38" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="1" t="n">
         <v>113.0123138</v>
       </c>
-      <c r="J38" s="1" t="n">
+      <c r="K38" s="1" t="n">
         <v>24.79294243</v>
       </c>
-      <c r="K38" s="1" t="n">
+      <c r="L38" s="1" t="n">
         <v>451.5821744</v>
       </c>
-      <c r="L38" s="1" t="n">
+      <c r="M38" s="1" t="n">
         <v>18.21414201</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>2019</v>
@@ -4108,21 +4234,24 @@
         <v>100</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="1" t="n">
+      <c r="I39" s="1" t="n">
         <v>11.0821467688938</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>2019</v>
@@ -4134,21 +4263,24 @@
         <v>300</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="1" t="n">
         <v>34.1347517730496</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>2019</v>
@@ -4160,30 +4292,33 @@
         <v>490</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H41" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41" s="1" t="n">
         <v>7.636546026</v>
       </c>
-      <c r="J41" s="1" t="n">
+      <c r="K41" s="1" t="n">
         <v>20.67419312</v>
       </c>
-      <c r="K41" s="1" t="n">
+      <c r="L41" s="1" t="n">
         <v>245.6279172</v>
       </c>
-      <c r="L41" s="1" t="n">
+      <c r="M41" s="1" t="n">
         <v>11.88089498</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>2019</v>
@@ -4195,21 +4330,24 @@
         <v>390</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H42" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I42" s="1" t="n">
         <v>20.82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>2019</v>
@@ -4221,33 +4359,36 @@
         <v>90</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" s="1" t="n">
         <v>80.48056313</v>
       </c>
-      <c r="I43" s="1" t="n">
+      <c r="J43" s="1" t="n">
         <v>4.62063615205586</v>
       </c>
-      <c r="J43" s="1" t="n">
+      <c r="K43" s="1" t="n">
         <v>353.5566298</v>
       </c>
-      <c r="K43" s="1" t="n">
+      <c r="L43" s="1" t="n">
         <v>1558.049231</v>
       </c>
-      <c r="L43" s="1" t="n">
+      <c r="M43" s="1" t="n">
         <v>4.406788334</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>2019</v>
@@ -4259,21 +4400,24 @@
         <v>490</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" s="1" t="n">
         <v>38.5986842105263</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>2019</v>
@@ -4285,21 +4429,24 @@
         <v>90</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" s="1" t="n">
         <v>21.2470308788599</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>2019</v>
@@ -4311,30 +4458,33 @@
         <v>520</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="1" t="n">
+      <c r="I46" s="1" t="n">
         <v>90.16563147</v>
       </c>
-      <c r="J46" s="1" t="n">
+      <c r="K46" s="1" t="n">
         <v>86.81522804</v>
       </c>
-      <c r="K46" s="1" t="n">
+      <c r="L46" s="1" t="n">
         <v>332.7506362</v>
       </c>
-      <c r="L46" s="1" t="n">
+      <c r="M46" s="1" t="n">
         <v>3.832860245</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>2019</v>
@@ -4346,21 +4496,24 @@
         <v>520</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="1" t="n">
         <v>18.495867768595</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>2019</v>
@@ -4372,33 +4525,36 @@
         <v>278</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H48" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="1" t="n">
         <v>53.0177949</v>
       </c>
-      <c r="I48" s="1" t="n">
+      <c r="J48" s="1" t="n">
         <v>13.5171898355755</v>
       </c>
-      <c r="J48" s="1" t="n">
+      <c r="K48" s="1" t="n">
         <v>52.99719101</v>
       </c>
-      <c r="K48" s="1" t="n">
+      <c r="L48" s="1" t="n">
         <v>204.4910401</v>
       </c>
-      <c r="L48" s="1" t="n">
+      <c r="M48" s="1" t="n">
         <v>3.858526013</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>2019</v>
@@ -4410,33 +4566,36 @@
         <v>107</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H49" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" s="1" t="n">
         <v>64.2526999</v>
       </c>
-      <c r="I49" s="1" t="n">
+      <c r="J49" s="1" t="n">
         <v>11.9092872570194</v>
       </c>
-      <c r="J49" s="1" t="n">
+      <c r="K49" s="1" t="n">
         <v>16.55766079</v>
       </c>
-      <c r="K49" s="1" t="n">
+      <c r="L49" s="1" t="n">
         <v>272.0780859</v>
       </c>
-      <c r="L49" s="1" t="n">
+      <c r="M49" s="1" t="n">
         <v>16.43215725</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>2019</v>
@@ -4448,21 +4607,24 @@
         <v>107</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H50" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I50" s="1" t="n">
         <v>13.1277997364954</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>2019</v>
@@ -4474,33 +4636,36 @@
         <v>107</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51" s="1" t="n">
         <v>23.8048780487805</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4525,7 +4690,7 @@
       <selection pane="topLeft" activeCell="S39" activeCellId="0" sqref="S39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>
@@ -4537,18 +4702,18 @@
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>102</v>
@@ -4563,7 +4728,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>130</v>
@@ -4578,7 +4743,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>170</v>
@@ -4593,7 +4758,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>300</v>
@@ -4608,7 +4773,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>370</v>
@@ -4623,7 +4788,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>570</v>
@@ -4638,7 +4803,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>700</v>
@@ -4653,7 +4818,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>770</v>
@@ -4668,7 +4833,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>965</v>
@@ -4686,18 +4851,18 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>90</v>
@@ -4712,7 +4877,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>100</v>
@@ -4727,7 +4892,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>107</v>
@@ -4742,7 +4907,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>171</v>
@@ -4757,7 +4922,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>173</v>
@@ -4772,7 +4937,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>200</v>
@@ -4787,7 +4952,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>278</v>
@@ -4802,7 +4967,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>300</v>
@@ -4817,7 +4982,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>402</v>
@@ -4832,7 +4997,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>490</v>
@@ -4847,7 +5012,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>520</v>
@@ -4862,7 +5027,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>965</v>
@@ -4920,18 +5085,18 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>170</v>
@@ -4940,15 +5105,15 @@
         <v>170</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>170</v>
@@ -4957,7 +5122,7 @@
         <v>170</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>202.5483083</v>
@@ -4969,10 +5134,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>570</v>
@@ -4981,15 +5146,15 @@
         <v>570</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>570</v>
@@ -4998,7 +5163,7 @@
         <v>570</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>52.53922915</v>
@@ -5010,10 +5175,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>570</v>
@@ -5022,15 +5187,15 @@
         <v>570</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>370</v>
@@ -5039,15 +5204,15 @@
         <v>370</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>370</v>
@@ -5056,7 +5221,7 @@
         <v>370</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>14.70959842</v>
@@ -5068,10 +5233,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>370</v>
@@ -5080,15 +5245,15 @@
         <v>370</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>102</v>
@@ -5097,15 +5262,15 @@
         <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>102</v>
@@ -5114,7 +5279,7 @@
         <v>102</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>120.2948594</v>
@@ -5126,10 +5291,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>102</v>
@@ -5138,15 +5303,15 @@
         <v>102</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>770</v>
@@ -5155,7 +5320,7 @@
         <v>770</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>41.23605442</v>
@@ -5167,10 +5332,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>770</v>
@@ -5179,15 +5344,15 @@
         <v>770</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>770</v>
@@ -5196,15 +5361,15 @@
         <v>770</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>130</v>
@@ -5213,7 +5378,7 @@
         <v>130</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>83.36974729</v>
@@ -5225,10 +5390,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>130</v>
@@ -5237,15 +5402,15 @@
         <v>130</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>130</v>
@@ -5254,15 +5419,15 @@
         <v>130</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>300</v>
@@ -5271,7 +5436,7 @@
         <v>300</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>43.50938879</v>
@@ -5283,10 +5448,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>700</v>
@@ -5295,7 +5460,7 @@
         <v>700</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>86.57859897</v>
@@ -5307,10 +5472,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>700</v>
@@ -5319,15 +5484,15 @@
         <v>700</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>700</v>
@@ -5336,15 +5501,15 @@
         <v>700</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>965</v>
@@ -5353,7 +5518,7 @@
         <v>965</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>69.3490879</v>
@@ -5365,10 +5530,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>965</v>
@@ -5377,15 +5542,15 @@
         <v>965</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>965</v>
@@ -5394,7 +5559,7 @@
         <v>965</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5414,18 +5579,18 @@
         <v>5</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>173</v>
@@ -5434,7 +5599,7 @@
         <v>173</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>154.782931</v>
@@ -5446,10 +5611,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>173</v>
@@ -5458,15 +5623,15 @@
         <v>173</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>173</v>
@@ -5475,15 +5640,15 @@
         <v>173</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>965</v>
@@ -5492,7 +5657,7 @@
         <v>965</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>186.4108454</v>
@@ -5504,10 +5669,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>402</v>
@@ -5516,15 +5681,15 @@
         <v>402</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>402</v>
@@ -5533,7 +5698,7 @@
         <v>402</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>398.5595814</v>
@@ -5545,10 +5710,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>171</v>
@@ -5557,7 +5722,7 @@
         <v>171</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>96.27078959</v>
@@ -5569,10 +5734,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>200</v>
@@ -5581,15 +5746,15 @@
         <v>200</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>200</v>
@@ -5598,7 +5763,7 @@
         <v>200</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>187.1856453</v>
@@ -5610,10 +5775,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>100</v>
@@ -5622,15 +5787,15 @@
         <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>300</v>
@@ -5639,7 +5804,7 @@
         <v>300</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F37" s="1" t="n">
         <v>363.0646116</v>
@@ -5651,10 +5816,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>300</v>
@@ -5663,15 +5828,15 @@
         <v>300</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>100</v>
@@ -5680,7 +5845,7 @@
         <v>100</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1" t="n">
         <v>451.5821744</v>
@@ -5692,10 +5857,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>100</v>
@@ -5704,15 +5869,15 @@
         <v>100</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>300</v>
@@ -5721,15 +5886,15 @@
         <v>300</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>490</v>
@@ -5738,7 +5903,7 @@
         <v>490</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>245.6279172</v>
@@ -5750,10 +5915,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>390</v>
@@ -5762,15 +5927,15 @@
         <v>390</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>90</v>
@@ -5779,7 +5944,7 @@
         <v>90</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>1558.049231</v>
@@ -5791,10 +5956,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>490</v>
@@ -5803,15 +5968,15 @@
         <v>490</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>90</v>
@@ -5820,15 +5985,15 @@
         <v>90</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>520</v>
@@ -5837,7 +6002,7 @@
         <v>520</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>332.7506362</v>
@@ -5849,10 +6014,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>520</v>
@@ -5861,15 +6026,15 @@
         <v>520</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>278</v>
@@ -5878,7 +6043,7 @@
         <v>278</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F49" s="1" t="n">
         <v>204.4910401</v>
@@ -5890,10 +6055,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>107</v>
@@ -5902,7 +6067,7 @@
         <v>107</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F50" s="1" t="n">
         <v>272.0780859</v>
@@ -5914,10 +6079,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>107</v>
@@ -5926,15 +6091,15 @@
         <v>107</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>107</v>
@@ -5943,27 +6108,27 @@
         <v>107</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
input 2018 2017 2019 inc in flux excels
</commit_message>
<xml_diff>
--- a/data/flux/2019-fluxes.xlsx
+++ b/data/flux/2019-fluxes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="88">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -108,12 +108,12 @@
     <t xml:space="preserve">top</t>
   </si>
   <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-58_370m_ctl</t>
   </si>
   <si>
-    <t xml:space="preserve">none</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-58_370m_+P</t>
   </si>
   <si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">4-59_300m_Fe_top_split</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fe</t>
   </si>
   <si>
     <t xml:space="preserve">4-59_700m_NO2_+P</t>
@@ -463,7 +460,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart85.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -646,11 +643,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="96207436"/>
-        <c:axId val="76600765"/>
+        <c:axId val="19437610"/>
+        <c:axId val="74337701"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96207436"/>
+        <c:axId val="19437610"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,12 +703,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76600765"/>
+        <c:crossAx val="74337701"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76600765"/>
+        <c:axId val="74337701"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -776,7 +773,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96207436"/>
+        <c:crossAx val="19437610"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -824,7 +821,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart86.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1025,11 +1022,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="12901862"/>
-        <c:axId val="93327045"/>
+        <c:axId val="5963184"/>
+        <c:axId val="56062989"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="12901862"/>
+        <c:axId val="5963184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1085,12 +1082,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93327045"/>
+        <c:crossAx val="56062989"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93327045"/>
+        <c:axId val="56062989"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1155,7 +1152,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12901862"/>
+        <c:crossAx val="5963184"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1203,7 +1200,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart87.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1419,11 +1416,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99072178"/>
-        <c:axId val="46759747"/>
+        <c:axId val="51693508"/>
+        <c:axId val="18813982"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99072178"/>
+        <c:axId val="51693508"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,12 +1476,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46759747"/>
+        <c:crossAx val="18813982"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46759747"/>
+        <c:axId val="18813982"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1549,7 +1546,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99072178"/>
+        <c:crossAx val="51693508"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,7 +1594,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart88.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1798,11 +1795,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="30431186"/>
-        <c:axId val="20768676"/>
+        <c:axId val="58340294"/>
+        <c:axId val="76890138"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30431186"/>
+        <c:axId val="58340294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,12 +1855,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20768676"/>
+        <c:crossAx val="76890138"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20768676"/>
+        <c:axId val="76890138"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1928,7 +1925,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30431186"/>
+        <c:crossAx val="58340294"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1976,7 +1973,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart89.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2193,11 +2190,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="77155396"/>
-        <c:axId val="30072250"/>
+        <c:axId val="84603619"/>
+        <c:axId val="50218208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77155396"/>
+        <c:axId val="84603619"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,12 +2250,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30072250"/>
+        <c:crossAx val="50218208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30072250"/>
+        <c:axId val="50218208"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2314,7 +2311,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77155396"/>
+        <c:crossAx val="84603619"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2341,7 +2338,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart90.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2567,11 +2564,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9467864"/>
-        <c:axId val="57914908"/>
+        <c:axId val="52753049"/>
+        <c:axId val="40653559"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9467864"/>
+        <c:axId val="52753049"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2627,12 +2624,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57914908"/>
+        <c:crossAx val="40653559"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57914908"/>
+        <c:axId val="40653559"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2688,7 +2685,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9467864"/>
+        <c:crossAx val="52753049"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2912,8 +2909,8 @@
   </sheetPr>
   <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H50" activeCellId="0" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3136,7 +3133,7 @@
         <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>9.72617743702081</v>
@@ -3144,7 +3141,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
@@ -3165,7 +3162,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>1.85815047021944</v>
@@ -3194,7 +3191,7 @@
         <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>19.66438915</v>
@@ -3235,7 +3232,7 @@
         <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>6.57961447055717</v>
@@ -3264,7 +3261,7 @@
         <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>24.9704142011834</v>
@@ -3293,7 +3290,7 @@
         <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>31.44875954</v>
@@ -3334,7 +3331,7 @@
         <v>27</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>9.5391061452514</v>
@@ -3363,7 +3360,7 @@
         <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>20.11954101</v>
@@ -3404,7 +3401,7 @@
         <v>27</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>11.0183881064163</v>
@@ -3433,7 +3430,7 @@
         <v>39</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>7.13300230537329</v>
@@ -3529,7 +3526,7 @@
         <v>27</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I18" s="1" t="n">
         <v>25.396694214876</v>
@@ -3558,7 +3555,7 @@
         <v>27</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="I19" s="1" t="n">
         <v>82.77252678</v>
@@ -3578,7 +3575,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
@@ -3619,7 +3616,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
@@ -3640,7 +3637,7 @@
         <v>27</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>11.1135940409683</v>
@@ -3648,7 +3645,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
@@ -3677,7 +3674,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
@@ -3698,7 +3695,7 @@
         <v>27</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>51.08955421</v>
@@ -3715,7 +3712,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>18</v>
@@ -3736,7 +3733,7 @@
         <v>23</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I24" s="1" t="n">
         <v>12.3266761768902</v>
@@ -3744,7 +3741,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>18</v>
@@ -3765,7 +3762,7 @@
         <v>20</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I25" s="1" t="n">
         <v>35.8697318007663</v>
@@ -3773,10 +3770,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>2019</v>
@@ -3794,7 +3791,7 @@
         <v>23</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>53.1000796</v>
@@ -3811,10 +3808,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>2019</v>
@@ -3832,7 +3829,7 @@
         <v>20</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>29.8271604938272</v>
@@ -3840,10 +3837,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2019</v>
@@ -3861,7 +3858,7 @@
         <v>27</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I28" s="1" t="n">
         <v>14.1515151515152</v>
@@ -3869,10 +3866,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2019</v>
@@ -3887,10 +3884,10 @@
         <v>19</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I29" s="1" t="n">
         <v>21.16318464</v>
@@ -3910,10 +3907,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>2019</v>
@@ -3931,7 +3928,7 @@
         <v>20</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I30" s="1" t="n">
         <v>30.1541353383459</v>
@@ -3939,10 +3936,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>2019</v>
@@ -3960,7 +3957,7 @@
         <v>27</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I31" s="1" t="n">
         <v>39.80676329</v>
@@ -3977,10 +3974,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>2019</v>
@@ -3998,7 +3995,7 @@
         <v>23</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I32" s="1" t="n">
         <v>49.79986197</v>
@@ -4015,10 +4012,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>2019</v>
@@ -4036,7 +4033,7 @@
         <v>20</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>28.9488188976378</v>
@@ -4044,10 +4041,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>2019</v>
@@ -4065,7 +4062,7 @@
         <v>27</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>82.99516908</v>
@@ -4085,10 +4082,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>2019</v>
@@ -4114,10 +4111,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>2019</v>
@@ -4135,7 +4132,7 @@
         <v>27</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>107.1438958</v>
@@ -4152,10 +4149,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>2019</v>
@@ -4181,10 +4178,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>2019</v>
@@ -4202,7 +4199,7 @@
         <v>27</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>113.0123138</v>
@@ -4219,10 +4216,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>2019</v>
@@ -4248,10 +4245,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>2019</v>
@@ -4277,10 +4274,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>2019</v>
@@ -4295,10 +4292,10 @@
         <v>19</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>7.636546026</v>
@@ -4315,10 +4312,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>2019</v>
@@ -4336,7 +4333,7 @@
         <v>27</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I42" s="1" t="n">
         <v>20.82</v>
@@ -4344,10 +4341,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>2019</v>
@@ -4365,7 +4362,7 @@
         <v>23</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I43" s="1" t="n">
         <v>80.48056313</v>
@@ -4385,10 +4382,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>2019</v>
@@ -4406,7 +4403,7 @@
         <v>20</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I44" s="1" t="n">
         <v>38.5986842105263</v>
@@ -4414,10 +4411,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>2019</v>
@@ -4435,7 +4432,7 @@
         <v>20</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I45" s="1" t="n">
         <v>21.2470308788599</v>
@@ -4443,10 +4440,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>2019</v>
@@ -4481,10 +4478,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>2019</v>
@@ -4510,10 +4507,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>2019</v>
@@ -4531,7 +4528,7 @@
         <v>23</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>53.0177949</v>
@@ -4551,10 +4548,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>2019</v>
@@ -4572,7 +4569,7 @@
         <v>23</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I49" s="1" t="n">
         <v>64.2526999</v>
@@ -4592,10 +4589,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>2019</v>
@@ -4613,7 +4610,7 @@
         <v>27</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I50" s="1" t="n">
         <v>13.1277997364954</v>
@@ -4621,10 +4618,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>2019</v>
@@ -4642,7 +4639,7 @@
         <v>20</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I51" s="1" t="n">
         <v>23.8048780487805</v>
@@ -4650,22 +4647,22 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4702,13 +4699,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4851,18 +4848,18 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="D12" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>90</v>
@@ -4877,7 +4874,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>100</v>
@@ -4892,7 +4889,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>107</v>
@@ -4907,7 +4904,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>171</v>
@@ -4922,7 +4919,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>173</v>
@@ -4937,7 +4934,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>200</v>
@@ -4952,7 +4949,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>278</v>
@@ -4967,7 +4964,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>300</v>
@@ -4982,7 +4979,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>402</v>
@@ -4997,7 +4994,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>490</v>
@@ -5012,7 +5009,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>520</v>
@@ -5027,7 +5024,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>965</v>
@@ -5088,7 +5085,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5192,7 +5189,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
@@ -5448,7 +5445,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
@@ -5472,7 +5469,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
@@ -5489,7 +5486,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
@@ -5506,7 +5503,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
@@ -5530,7 +5527,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>18</v>
@@ -5547,7 +5544,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>18</v>
@@ -5582,15 +5579,15 @@
         <v>11</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>173</v>
@@ -5611,10 +5608,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>173</v>
@@ -5628,10 +5625,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>173</v>
@@ -5645,10 +5642,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>965</v>
@@ -5669,10 +5666,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>402</v>
@@ -5686,10 +5683,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>402</v>
@@ -5710,10 +5707,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>171</v>
@@ -5734,10 +5731,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>200</v>
@@ -5751,10 +5748,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>200</v>
@@ -5775,10 +5772,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>100</v>
@@ -5792,10 +5789,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>300</v>
@@ -5816,10 +5813,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>300</v>
@@ -5833,10 +5830,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>100</v>
@@ -5857,10 +5854,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>100</v>
@@ -5874,10 +5871,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>300</v>
@@ -5891,10 +5888,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>490</v>
@@ -5915,10 +5912,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>390</v>
@@ -5932,10 +5929,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>90</v>
@@ -5956,10 +5953,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>490</v>
@@ -5973,10 +5970,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>90</v>
@@ -5990,10 +5987,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>520</v>
@@ -6014,10 +6011,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>520</v>
@@ -6031,10 +6028,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>278</v>
@@ -6055,10 +6052,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>107</v>
@@ -6079,10 +6076,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>107</v>
@@ -6096,10 +6093,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>107</v>
@@ -6113,22 +6110,22 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>